<commit_message>
fixed sync issue with search post.
</commit_message>
<xml_diff>
--- a/my-tests/src/main/resources/dataSheets/testData_Avner.xlsx
+++ b/my-tests/src/main/resources/dataSheets/testData_Avner.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26408"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AvnerG\workspace\my-tests\src\main\resources\dataSheets\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/avner/git/my-tests/my-tests/src/main/resources/dataSheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11610" windowHeight="7080" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="devices (2)" sheetId="21" r:id="rId1"/>
@@ -17,9 +17,12 @@
     <sheet name="signIn" sheetId="18" r:id="rId3"/>
     <sheet name="findPost" sheetId="20" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -27,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
   <si>
     <t>deviceName</t>
   </si>
@@ -98,9 +101,6 @@
     <t>xxxxxxx</t>
   </si>
   <si>
-    <t>Hi Someone!</t>
-  </si>
-  <si>
     <t>firefox</t>
   </si>
   <si>
@@ -140,28 +140,7 @@
     <t>postIndex</t>
   </si>
   <si>
-    <t>mobileOS</t>
-  </si>
-  <si>
-    <t>iphone-6</t>
-  </si>
-  <si>
-    <t>Galaxy S5</t>
-  </si>
-  <si>
-    <t>iPad Air 2</t>
-  </si>
-  <si>
-    <t>Shared</t>
-  </si>
-  <si>
-    <t>Brian</t>
-  </si>
-  <si>
-    <t>Chrome</t>
-  </si>
-  <si>
-    <t>887544662</t>
+    <t>Hi, Avner!</t>
   </si>
 </sst>
 </file>
@@ -501,26 +480,26 @@
   <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J7" sqref="J7"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.5703125" customWidth="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -558,7 +537,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E2" t="s">
         <v>11</v>
       </c>
@@ -569,7 +548,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E3" t="s">
         <v>11</v>
       </c>
@@ -580,19 +559,19 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="D6" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="D6" t="s">
-        <v>26</v>
       </c>
       <c r="I6" t="s">
         <v>18</v>
@@ -609,29 +588,29 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I6" sqref="I6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.6640625" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -669,47 +648,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E4" t="s">
-        <v>38</v>
-      </c>
-      <c r="I4" t="s">
-        <v>18</v>
-      </c>
-      <c r="J4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E5" t="s">
-        <v>39</v>
-      </c>
-      <c r="I5" t="s">
-        <v>42</v>
-      </c>
-      <c r="J5" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="E6" t="s">
-        <v>40</v>
-      </c>
-      <c r="I6" t="s">
-        <v>41</v>
-      </c>
-      <c r="J6" t="s">
-        <v>37</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -720,20 +661,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.140625" customWidth="1"/>
+    <col min="1" max="1" width="28.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>12</v>
       </c>
@@ -744,7 +685,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -752,36 +693,24 @@
         <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1"/>
     <hyperlink ref="A3" r:id="rId2"/>
-    <hyperlink ref="A4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="75" verticalDpi="75" r:id="rId4"/>
+  <pageSetup orientation="portrait" horizontalDpi="75" verticalDpi="75" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -793,66 +722,66 @@
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="49" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>29</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>34</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor sync tweaks to the POM package.
</commit_message>
<xml_diff>
--- a/my-tests/src/main/resources/dataSheets/testData_Avner.xlsx
+++ b/my-tests/src/main/resources/dataSheets/testData_Avner.xlsx
@@ -9,13 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19760" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="19760"/>
   </bookViews>
   <sheets>
-    <sheet name="devices (2)" sheetId="21" r:id="rId1"/>
-    <sheet name="devices" sheetId="19" r:id="rId2"/>
-    <sheet name="signIn" sheetId="18" r:id="rId3"/>
-    <sheet name="findPost" sheetId="20" r:id="rId4"/>
+    <sheet name="devices" sheetId="21" r:id="rId1"/>
+    <sheet name="signIn" sheetId="18" r:id="rId2"/>
+    <sheet name="findPost" sheetId="20" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="39">
   <si>
     <t>deviceName</t>
   </si>
@@ -86,61 +85,67 @@
     <t>appPackage</t>
   </si>
   <si>
-    <t>Avner</t>
-  </si>
-  <si>
     <t>MobileOS</t>
   </si>
   <si>
-    <t>Raj</t>
-  </si>
-  <si>
     <t>wrongEmail@gmail.com</t>
   </si>
   <si>
     <t>xxxxxxx</t>
   </si>
   <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>Samsung</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>postTitle</t>
+  </si>
+  <si>
+    <t>fluent wait</t>
+  </si>
+  <si>
+    <t>testng</t>
+  </si>
+  <si>
+    <t>ci</t>
+  </si>
+  <si>
+    <t>Selenium wait for object</t>
+  </si>
+  <si>
+    <t>Manage TestNG execution and Data</t>
+  </si>
+  <si>
+    <t>jenkins setup</t>
+  </si>
+  <si>
+    <t>Jenkins TomCat Setup as a Windows Service – CI Automation</t>
+  </si>
+  <si>
+    <t>postIndex</t>
+  </si>
+  <si>
+    <t>Hi, Avner!</t>
+  </si>
+  <si>
+    <t>Avner|Raj|Brian</t>
+  </si>
+  <si>
+    <t>Avner|raj|Brian</t>
+  </si>
+  <si>
     <t>firefox</t>
   </si>
   <si>
-    <t>chrome</t>
-  </si>
-  <si>
-    <t>Samsung</t>
-  </si>
-  <si>
-    <t>q</t>
-  </si>
-  <si>
-    <t>postTitle</t>
-  </si>
-  <si>
-    <t>fluent wait</t>
-  </si>
-  <si>
-    <t>testng</t>
-  </si>
-  <si>
-    <t>ci</t>
-  </si>
-  <si>
-    <t>Selenium wait for object</t>
-  </si>
-  <si>
-    <t>Manage TestNG execution and Data</t>
-  </si>
-  <si>
-    <t>jenkins setup</t>
-  </si>
-  <si>
-    <t>Jenkins TomCat Setup as a Windows Service – CI Automation</t>
-  </si>
-  <si>
-    <t>postIndex</t>
-  </si>
-  <si>
-    <t>Hi, Avner!</t>
+    <t>iPad*.*</t>
+  </si>
+  <si>
+    <t>Shared</t>
   </si>
 </sst>
 </file>
@@ -479,8 +484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -542,42 +547,42 @@
         <v>11</v>
       </c>
       <c r="I2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" t="s">
         <v>18</v>
       </c>
-      <c r="J2" t="s">
-        <v>19</v>
-      </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E3" t="s">
-        <v>11</v>
+      <c r="D3" t="s">
+        <v>22</v>
       </c>
       <c r="I3" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="J3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="D6" t="s">
-        <v>25</v>
+      <c r="E6" t="s">
+        <v>37</v>
       </c>
       <c r="I6" t="s">
+        <v>38</v>
+      </c>
+      <c r="J6" t="s">
         <v>18</v>
-      </c>
-      <c r="J6" t="s">
-        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -587,79 +592,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="19" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="8.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="18.6640625" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="13.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="14.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -693,15 +625,15 @@
         <v>16</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -714,7 +646,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
@@ -731,57 +663,57 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B4">
         <v>2</v>
       </c>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B5">
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>